<commit_message>
Added indication LED. Generated CAM files. Generated BoM and PnP files.
</commit_message>
<xml_diff>
--- a/cam/DCDC-12V5V5A_2021-07-25-BoM.xlsx
+++ b/cam/DCDC-12V5V5A_2021-07-25-BoM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DCDC\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF30B2F-9065-46CE-9F1D-309865013DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CE056E-AC2D-47A4-A424-74B8629D75FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="550" windowWidth="17320" windowHeight="19950" xr2:uid="{A450ADA1-A548-498C-850B-47BCE1D33AA2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$1:$D$14</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$1:$D$15</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>Qty</t>
   </si>
@@ -80,9 +80,6 @@
     <t>3k</t>
   </si>
   <si>
-    <t>R18, R19</t>
-  </si>
-  <si>
     <t>470nF</t>
   </si>
   <si>
@@ -189,6 +186,21 @@
   </si>
   <si>
     <t>TO-252-2</t>
+  </si>
+  <si>
+    <t>R1, R18, R19</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>LED_0603</t>
+  </si>
+  <si>
+    <t>C72043</t>
+  </si>
+  <si>
+    <t>GREEN</t>
   </si>
 </sst>
 </file>
@@ -317,8 +329,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F615F04-3A29-4709-9576-D28F831230BE}" name="DCDC_12V5V5A" displayName="DCDC_12V5V5A" ref="A1:E14" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E14" xr:uid="{0F615F04-3A29-4709-9576-D28F831230BE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F615F04-3A29-4709-9576-D28F831230BE}" name="DCDC_12V5V5A" displayName="DCDC_12V5V5A" ref="A1:E15" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:E15" xr:uid="{0F615F04-3A29-4709-9576-D28F831230BE}"/>
   <tableColumns count="5">
     <tableColumn id="39" xr3:uid="{09F6E98D-07FB-41A6-BAC3-A39CA2127826}" uniqueName="39" name="Qty" queryTableFieldId="1"/>
     <tableColumn id="41" xr3:uid="{B76CEAED-081C-4D83-8673-E56B36213B08}" uniqueName="41" name="Designator" queryTableFieldId="40" dataDxfId="3"/>
@@ -627,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFDA44F-A04D-4249-BA0F-9AE7E1F271E9}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -648,16 +660,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -668,13 +680,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -685,13 +697,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -702,13 +714,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -719,13 +731,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -736,13 +748,13 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -753,30 +765,30 @@
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -784,16 +796,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -801,16 +813,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -818,16 +830,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -835,16 +847,16 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -852,16 +864,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -869,16 +881,33 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor improvements in board routing. Generated CAM files. Fixed footprints in BoM.
</commit_message>
<xml_diff>
--- a/cam/DCDC-12V5V5A_2021-07-25-BoM.xlsx
+++ b/cam/DCDC-12V5V5A_2021-07-25-BoM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DCDC\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CE056E-AC2D-47A4-A424-74B8629D75FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04336135-EA09-4C79-A288-FBF65753152A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="550" windowWidth="17320" windowHeight="19950" xr2:uid="{A450ADA1-A548-498C-850B-47BCE1D33AA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Qty</t>
   </si>
@@ -123,12 +123,6 @@
   </si>
   <si>
     <t>0603</t>
-  </si>
-  <si>
-    <t>0604</t>
-  </si>
-  <si>
-    <t>0605</t>
   </si>
   <si>
     <t>0805</t>
@@ -642,7 +636,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -669,7 +663,7 @@
         <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -686,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -697,13 +691,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -714,13 +708,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -731,13 +725,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -754,7 +748,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -765,13 +759,13 @@
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -779,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>28</v>
@@ -788,7 +782,7 @@
         <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -805,7 +799,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -822,7 +816,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -839,7 +833,7 @@
         <v>18</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -856,7 +850,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -867,13 +861,13 @@
         <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -884,13 +878,13 @@
         <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -898,16 +892,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>